<commit_message>
adding external repo code
</commit_message>
<xml_diff>
--- a/experiments/compas/results/all_results.xlsx
+++ b/experiments/compas/results/all_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ancarey\PycharmProjects\adaptive-hypernets\experiments\compas\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E94C9-AD04-4BD8-A8D0-D20930185429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322BFE61-216F-46E1-9D92-CFEDFA299AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4524E15B-8C05-4645-AAC7-9D29869D5525}"/>
+    <workbookView xWindow="30240" yWindow="585" windowWidth="24960" windowHeight="14055" xr2:uid="{4524E15B-8C05-4645-AAC7-9D29869D5525}"/>
   </bookViews>
   <sheets>
     <sheet name="compas-one-client" sheetId="4" r:id="rId1"/>
@@ -591,13 +591,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -609,38 +627,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
@@ -650,18 +662,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91775286-5ED5-4E96-8261-8DCB4AC2C91F}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH5" sqref="AH5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,74 +1008,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="27" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="42"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="30" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="31"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="30" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="30" t="s">
+      <c r="U1" s="37"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="27" t="s">
+      <c r="X1" s="37"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AA1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AB1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AC1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AD1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="AF1" s="39" t="s">
+      <c r="AF1" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="16" t="s">
         <v>25</v>
       </c>
@@ -1094,9 +1094,9 @@
       <c r="G2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
       <c r="K2" s="16" t="s">
         <v>25</v>
       </c>
@@ -1142,34 +1142,34 @@
       <c r="Y2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="27"/>
-      <c r="AF2" s="40"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="33"/>
+      <c r="AF2" s="29"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="C3" s="3">
         <v>0.68400000000000005</v>
       </c>
-      <c r="C3" s="3">
-        <v>0.68200000000000005</v>
-      </c>
       <c r="D3" s="3">
-        <v>0.68500000000000005</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="E3" s="3">
+        <v>0.313</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.316</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.318</v>
-      </c>
       <c r="G3" s="1">
-        <v>0.315</v>
+        <v>0.312</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>21</v>
@@ -1181,88 +1181,88 @@
         <v>17</v>
       </c>
       <c r="K3" s="6">
-        <v>161.80000000000001</v>
+        <v>157</v>
       </c>
       <c r="L3" s="6">
-        <v>19.3</v>
+        <v>18</v>
       </c>
       <c r="M3" s="6">
-        <v>142.5</v>
+        <v>139</v>
       </c>
       <c r="N3" s="6">
-        <v>71.599999999999994</v>
+        <v>65</v>
       </c>
       <c r="O3" s="6">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="P3" s="6">
-        <v>65.099999999999994</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="6">
-        <v>260.39999999999998</v>
+        <v>267</v>
       </c>
       <c r="R3" s="6">
-        <v>58.5</v>
+        <v>60</v>
       </c>
       <c r="S3" s="6">
-        <v>201.9</v>
+        <v>207</v>
       </c>
       <c r="T3" s="6">
-        <v>123.2</v>
+        <v>128</v>
       </c>
       <c r="U3" s="6">
-        <v>29.7</v>
+        <v>31</v>
       </c>
       <c r="V3" s="6">
-        <v>93.5</v>
+        <v>97</v>
       </c>
       <c r="W3" s="6">
-        <v>0.624</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="X3" s="6">
-        <v>0.51400000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="Y3" s="6">
-        <v>0.64200000000000002</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="Z3" s="6">
-        <v>0.63</v>
+        <v>0.66</v>
       </c>
       <c r="AA3" s="11">
-        <v>-0.2099</v>
+        <v>-0.22159999999999999</v>
       </c>
       <c r="AB3" s="11">
-        <v>-0.18640000000000001</v>
+        <v>-0.19389999999999999</v>
       </c>
       <c r="AC3" s="11">
-        <v>-0.1769</v>
+        <v>-0.1847</v>
       </c>
       <c r="AD3" s="6">
-        <v>5.31</v>
-      </c>
-      <c r="AF3" s="40"/>
+        <v>5.14</v>
+      </c>
+      <c r="AF3" s="29"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="7">
-        <v>0.68600000000000005</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="C4" s="7">
-        <v>0.68799999999999994</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="D4" s="7">
-        <v>0.68600000000000005</v>
+        <v>0.68</v>
       </c>
       <c r="E4" s="7">
-        <v>0.314</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="F4" s="7">
-        <v>0.312</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="G4" s="7">
-        <v>0.314</v>
+        <v>0.32</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>15</v>
@@ -1274,89 +1274,77 @@
         <v>17</v>
       </c>
       <c r="K4" s="7">
-        <v>165.9</v>
+        <v>164</v>
       </c>
       <c r="L4" s="7">
-        <v>21.6</v>
+        <v>20</v>
       </c>
       <c r="M4" s="7">
-        <v>144.30000000000001</v>
+        <v>144</v>
       </c>
       <c r="N4" s="7">
-        <v>74.5</v>
+        <v>77</v>
       </c>
       <c r="O4" s="7">
-        <v>8.1999999999999993</v>
+        <v>8</v>
       </c>
       <c r="P4" s="7">
-        <v>66.3</v>
+        <v>69</v>
       </c>
       <c r="Q4" s="7">
-        <v>257.5</v>
+        <v>255</v>
       </c>
       <c r="R4" s="7">
-        <v>56.8</v>
+        <v>57</v>
       </c>
       <c r="S4" s="7">
-        <v>200.7</v>
+        <v>198</v>
       </c>
       <c r="T4" s="7">
-        <v>119.1</v>
+        <v>121</v>
       </c>
       <c r="U4" s="7">
-        <v>27.4</v>
+        <v>29</v>
       </c>
       <c r="V4" s="7">
-        <v>91.7</v>
+        <v>92</v>
       </c>
       <c r="W4" s="7">
-        <v>0.63100000000000001</v>
+        <v>0.624</v>
       </c>
       <c r="X4" s="7">
-        <v>0.54800000000000004</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="Y4" s="7">
-        <v>0.64600000000000002</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="Z4" s="7">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="AA4" s="13">
-        <v>-0.1706</v>
+        <v>-0.20200000000000001</v>
       </c>
       <c r="AB4" s="13">
-        <v>-0.1573</v>
+        <v>-0.17780000000000001</v>
       </c>
       <c r="AC4" s="13">
-        <v>-0.1464</v>
+        <v>-0.16869999999999999</v>
       </c>
       <c r="AD4" s="7">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="AF4" s="40"/>
+        <v>8.24</v>
+      </c>
+      <c r="AF4" s="29"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.314</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.312</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
@@ -1366,67 +1354,27 @@
       <c r="J5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="6">
-        <v>158.5</v>
-      </c>
-      <c r="L5" s="6">
-        <v>17</v>
-      </c>
-      <c r="M5" s="6">
-        <v>141.5</v>
-      </c>
-      <c r="N5" s="6">
-        <v>67.2</v>
-      </c>
-      <c r="O5" s="6">
-        <v>4.8</v>
-      </c>
-      <c r="P5" s="6">
-        <v>62.4</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>264.8</v>
-      </c>
-      <c r="R5" s="6">
-        <v>60.2</v>
-      </c>
-      <c r="S5" s="6">
-        <v>204.6</v>
-      </c>
-      <c r="T5" s="6">
-        <v>126.5</v>
-      </c>
-      <c r="U5" s="6">
-        <v>32</v>
-      </c>
-      <c r="V5" s="6">
-        <v>94.5</v>
-      </c>
-      <c r="W5" s="6">
-        <v>0.621</v>
-      </c>
-      <c r="X5" s="6">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="Y5" s="6">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="Z5" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="AA5" s="11">
-        <v>-0.25259999999999999</v>
-      </c>
-      <c r="AB5" s="11">
-        <v>-0.21410000000000001</v>
-      </c>
-      <c r="AC5" s="11">
-        <v>-0.20619999999999999</v>
-      </c>
-      <c r="AD5" s="6">
-        <v>7.35</v>
-      </c>
-      <c r="AF5" s="40"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="6"/>
+      <c r="AF5" s="29"/>
       <c r="AH5" t="s">
         <v>82</v>
       </c>
@@ -1435,24 +1383,12 @@
       <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.68</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0.317</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0.307</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0.32</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="10" t="s">
         <v>15</v>
       </c>
@@ -1462,90 +1398,38 @@
       <c r="J6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="9">
-        <v>163.80000000000001</v>
-      </c>
-      <c r="L6" s="9">
-        <v>21.2</v>
-      </c>
-      <c r="M6" s="9">
-        <v>142.6</v>
-      </c>
-      <c r="N6" s="9">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="O6" s="9">
-        <v>7.2</v>
-      </c>
-      <c r="P6" s="9">
-        <v>67.400000000000006</v>
-      </c>
-      <c r="Q6" s="9">
-        <v>257.39999999999998</v>
-      </c>
-      <c r="R6" s="9">
-        <v>57.8</v>
-      </c>
-      <c r="S6" s="9">
-        <v>199.6</v>
-      </c>
-      <c r="T6" s="9">
-        <v>121.2</v>
-      </c>
-      <c r="U6" s="9">
-        <v>27.8</v>
-      </c>
-      <c r="V6" s="9">
-        <v>93.4</v>
-      </c>
-      <c r="W6" s="9">
-        <v>0.626</v>
-      </c>
-      <c r="X6" s="9">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="Y6" s="9">
-        <v>0.63900000000000001</v>
-      </c>
-      <c r="Z6" s="9">
-        <v>0.64</v>
-      </c>
-      <c r="AA6" s="12">
-        <v>-0.1716</v>
-      </c>
-      <c r="AB6" s="12">
-        <v>-0.16839999999999999</v>
-      </c>
-      <c r="AC6" s="12">
-        <v>-0.15659999999999999</v>
-      </c>
-      <c r="AD6" s="9">
-        <v>9.73</v>
-      </c>
-      <c r="AF6" s="40"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="9"/>
+      <c r="AF6" s="29"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.316</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.314</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
         <v>33</v>
       </c>
@@ -1555,90 +1439,38 @@
       <c r="J7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="6">
-        <v>161</v>
-      </c>
-      <c r="L7" s="6">
-        <v>16.5</v>
-      </c>
-      <c r="M7" s="6">
-        <v>144.5</v>
-      </c>
-      <c r="N7" s="6">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="O7" s="6">
-        <v>4.7</v>
-      </c>
-      <c r="P7" s="6">
-        <v>66.2</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>261.10000000000002</v>
-      </c>
-      <c r="R7" s="6">
-        <v>60.3</v>
-      </c>
-      <c r="S7" s="6">
-        <v>200.8</v>
-      </c>
-      <c r="T7" s="6">
-        <v>124</v>
-      </c>
-      <c r="U7" s="6">
-        <v>32.5</v>
-      </c>
-      <c r="V7" s="6">
-        <v>91.5</v>
-      </c>
-      <c r="W7" s="6">
-        <v>0.623</v>
-      </c>
-      <c r="X7" s="6">
-        <v>0.47</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="AA7" s="11">
-        <v>-0.27560000000000001</v>
-      </c>
-      <c r="AB7" s="11">
-        <v>-0.2329</v>
-      </c>
-      <c r="AC7" s="11">
-        <v>-0.22559999999999999</v>
-      </c>
-      <c r="AD7" s="6">
-        <v>9.27</v>
-      </c>
-      <c r="AF7" s="40"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="6"/>
+      <c r="AF7" s="29"/>
     </row>
     <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="7">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="C8" s="7">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0.316</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0.32200000000000001</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="10" t="s">
         <v>39</v>
       </c>
@@ -1648,154 +1480,114 @@
       <c r="J8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="9">
-        <v>164</v>
-      </c>
-      <c r="L8" s="9">
-        <v>21</v>
-      </c>
-      <c r="M8" s="9">
-        <v>143</v>
-      </c>
-      <c r="N8" s="9">
-        <v>77</v>
-      </c>
-      <c r="O8" s="9">
-        <v>8</v>
-      </c>
-      <c r="P8" s="9">
-        <v>69</v>
-      </c>
-      <c r="Q8" s="9">
-        <v>255</v>
-      </c>
-      <c r="R8" s="9">
-        <v>57</v>
-      </c>
-      <c r="S8" s="9">
-        <v>198</v>
-      </c>
-      <c r="T8" s="9">
-        <v>121</v>
-      </c>
-      <c r="U8" s="9">
-        <v>28</v>
-      </c>
-      <c r="V8" s="9">
-        <v>93</v>
-      </c>
-      <c r="W8" s="9">
-        <v>0.622</v>
-      </c>
-      <c r="X8" s="9">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="Y8" s="9">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="Z8" s="9">
-        <v>0.66</v>
-      </c>
-      <c r="AA8" s="9">
-        <v>-0.1774</v>
-      </c>
-      <c r="AB8" s="9">
-        <v>-0.1671</v>
-      </c>
-      <c r="AC8" s="9">
-        <v>-0.15640000000000001</v>
-      </c>
-      <c r="AD8" s="9">
-        <v>98.24</v>
-      </c>
-      <c r="AF8" s="41"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AF8" s="30"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF9" s="19"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
     </row>
     <row r="11" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="30" t="s">
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="42" t="s">
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="27" t="s">
+      <c r="L12" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="34" t="s">
+      <c r="M12" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="N12" s="35"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="30" t="s">
+      <c r="N12" s="42"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="30" t="s">
+      <c r="Q12" s="37"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="T12" s="31"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="30" t="s">
+      <c r="T12" s="37"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="W12" s="31"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="30" t="s">
+      <c r="W12" s="37"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="Z12" s="31"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="27" t="s">
+      <c r="Z12" s="37"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="AC12" s="28" t="s">
+      <c r="AC12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AD12" s="28" t="s">
+      <c r="AD12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AE12" s="28" t="s">
+      <c r="AE12" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="AF12" s="27" t="s">
+      <c r="AF12" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="AH12" s="39" t="s">
+      <c r="AH12" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="17" t="s">
         <v>25</v>
       </c>
@@ -1814,11 +1606,11 @@
       <c r="G13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
       <c r="M13" s="17" t="s">
         <v>25</v>
       </c>
@@ -1864,12 +1656,12 @@
       <c r="AA13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="29"/>
-      <c r="AD13" s="29"/>
-      <c r="AE13" s="29"/>
-      <c r="AF13" s="27"/>
-      <c r="AH13" s="40"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="32"/>
+      <c r="AD13" s="32"/>
+      <c r="AE13" s="32"/>
+      <c r="AF13" s="33"/>
+      <c r="AH13" s="29"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
@@ -1968,7 +1760,7 @@
       <c r="AF14" s="6">
         <v>15.22</v>
       </c>
-      <c r="AH14" s="40"/>
+      <c r="AH14" s="29"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
@@ -2067,7 +1859,7 @@
       <c r="AF15" s="7">
         <v>13.54</v>
       </c>
-      <c r="AH15" s="40"/>
+      <c r="AH15" s="29"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
@@ -2166,7 +1958,7 @@
       <c r="AF16" s="6">
         <v>12.61</v>
       </c>
-      <c r="AH16" s="40"/>
+      <c r="AH16" s="29"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
@@ -2265,7 +2057,7 @@
       <c r="AF17" s="9">
         <v>15.31</v>
       </c>
-      <c r="AH17" s="40"/>
+      <c r="AH17" s="29"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
@@ -2364,7 +2156,7 @@
       <c r="AF18" s="6">
         <v>1.62</v>
       </c>
-      <c r="AH18" s="40"/>
+      <c r="AH18" s="29"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
@@ -2463,7 +2255,7 @@
       <c r="AF19" s="9">
         <v>22.7</v>
       </c>
-      <c r="AH19" s="40"/>
+      <c r="AH19" s="29"/>
     </row>
     <row r="20" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
@@ -2562,7 +2354,7 @@
       <c r="AF20" s="6">
         <v>1.61</v>
       </c>
-      <c r="AH20" s="40"/>
+      <c r="AH20" s="29"/>
     </row>
     <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
@@ -2661,15 +2453,26 @@
       <c r="AF21" s="9">
         <v>22.56</v>
       </c>
-      <c r="AH21" s="41"/>
+      <c r="AH21" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AH12:AH21"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="AD12:AD13"/>
-    <mergeCell ref="AE12:AE13"/>
-    <mergeCell ref="AF12:AF13"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
     <mergeCell ref="AF1:AF8"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:D12"/>
@@ -2686,22 +2489,11 @@
     <mergeCell ref="Y12:AA12"/>
     <mergeCell ref="AB12:AB13"/>
     <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AH12:AH21"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="AD12:AD13"/>
+    <mergeCell ref="AE12:AE13"/>
+    <mergeCell ref="AF12:AF13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2712,7 +2504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80701A8F-7759-45F4-A607-162CF246F76F}">
   <dimension ref="A1:BH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="BC8" sqref="BC8"/>
     </sheetView>
   </sheetViews>
@@ -2720,7 +2512,7 @@
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" style="27" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -2728,124 +2520,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="30" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="30" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="27" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="35"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="34" t="s">
+      <c r="R1" s="42"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="35"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="30" t="s">
+      <c r="U1" s="42"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="30" t="s">
+      <c r="X1" s="37"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="30" t="s">
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="30" t="s">
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="30" t="s">
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="30" t="s">
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="30" t="s">
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="30" t="s">
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="27" t="s">
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AV1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="AW1" s="28" t="s">
+      <c r="AW1" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="AX1" s="28" t="s">
+      <c r="AX1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="AY1" s="28" t="s">
+      <c r="AY1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AZ1" s="28" t="s">
+      <c r="AZ1" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="BA1" s="28" t="s">
+      <c r="BA1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BB1" s="28" t="s">
+      <c r="BB1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="BC1" s="27" t="s">
+      <c r="BC1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="BD1" s="27" t="s">
+      <c r="BD1" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="BF1" s="44" t="s">
+      <c r="BF1" s="48" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="22" t="s">
         <v>25</v>
       </c>
@@ -2882,9 +2674,9 @@
       <c r="M2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
       <c r="Q2" s="22" t="s">
         <v>25</v>
       </c>
@@ -2975,17 +2767,17 @@
       <c r="AT2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="29"/>
-      <c r="AX2" s="29"/>
-      <c r="AY2" s="29"/>
-      <c r="AZ2" s="29"/>
-      <c r="BA2" s="29"/>
-      <c r="BB2" s="29"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BF2" s="45"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="33"/>
+      <c r="BD2" s="33"/>
+      <c r="BF2" s="49"/>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -3156,7 +2948,7 @@
       <c r="BD3" s="6">
         <v>2.58</v>
       </c>
-      <c r="BF3" s="45"/>
+      <c r="BF3" s="49"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -3327,7 +3119,7 @@
       <c r="BD4" s="7">
         <v>4.1900000000000004</v>
       </c>
-      <c r="BF4" s="45"/>
+      <c r="BF4" s="49"/>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
@@ -3498,7 +3290,7 @@
       <c r="BD5" s="6">
         <v>3.76</v>
       </c>
-      <c r="BF5" s="45"/>
+      <c r="BF5" s="49"/>
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
@@ -3669,7 +3461,7 @@
       <c r="BD6" s="9">
         <v>4.87</v>
       </c>
-      <c r="BF6" s="45"/>
+      <c r="BF6" s="49"/>
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
@@ -3840,7 +3632,7 @@
       <c r="BD7" s="6">
         <v>3.55</v>
       </c>
-      <c r="BF7" s="45"/>
+      <c r="BF7" s="49"/>
     </row>
     <row r="8" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
@@ -3907,134 +3699,134 @@
       <c r="BB8" s="9"/>
       <c r="BC8" s="9"/>
       <c r="BD8" s="9"/>
-      <c r="BF8" s="46"/>
+      <c r="BF8" s="50"/>
     </row>
     <row r="11" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="30" t="s">
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="30" t="s">
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="30" t="s">
+      <c r="I12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="L12" s="31"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="42" t="s">
+      <c r="L12" s="37"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="O12" s="42" t="s">
+      <c r="O12" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="27" t="s">
+      <c r="Q12" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="R12" s="27" t="s">
+      <c r="R12" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="S12" s="34" t="s">
+      <c r="S12" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="T12" s="35"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="34" t="s">
+      <c r="T12" s="42"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="W12" s="35"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="30" t="s">
+      <c r="W12" s="42"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="Z12" s="31"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="30" t="s">
+      <c r="Z12" s="37"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="AC12" s="31"/>
-      <c r="AD12" s="32"/>
-      <c r="AE12" s="30" t="s">
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="38"/>
+      <c r="AE12" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="AF12" s="31"/>
-      <c r="AG12" s="32"/>
-      <c r="AH12" s="30" t="s">
+      <c r="AF12" s="37"/>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="AI12" s="31"/>
-      <c r="AJ12" s="32"/>
-      <c r="AK12" s="30" t="s">
+      <c r="AI12" s="37"/>
+      <c r="AJ12" s="38"/>
+      <c r="AK12" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="AL12" s="31"/>
-      <c r="AM12" s="32"/>
-      <c r="AN12" s="30" t="s">
+      <c r="AL12" s="37"/>
+      <c r="AM12" s="38"/>
+      <c r="AN12" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="AO12" s="31"/>
-      <c r="AP12" s="32"/>
-      <c r="AQ12" s="30" t="s">
+      <c r="AO12" s="37"/>
+      <c r="AP12" s="38"/>
+      <c r="AQ12" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AR12" s="31"/>
-      <c r="AS12" s="32"/>
-      <c r="AT12" s="30" t="s">
+      <c r="AR12" s="37"/>
+      <c r="AS12" s="38"/>
+      <c r="AT12" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="AU12" s="31"/>
-      <c r="AV12" s="32"/>
-      <c r="AW12" s="27" t="s">
+      <c r="AU12" s="37"/>
+      <c r="AV12" s="38"/>
+      <c r="AW12" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="AX12" s="27" t="s">
+      <c r="AX12" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="AY12" s="28" t="s">
+      <c r="AY12" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="AZ12" s="28" t="s">
+      <c r="AZ12" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="BA12" s="28" t="s">
+      <c r="BA12" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="BB12" s="28" t="s">
+      <c r="BB12" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="BC12" s="28" t="s">
+      <c r="BC12" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BD12" s="28" t="s">
+      <c r="BD12" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="BE12" s="27" t="s">
+      <c r="BE12" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="BF12" s="27" t="s">
+      <c r="BF12" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="BH12" s="47" t="s">
+      <c r="BH12" s="45" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="25" t="s">
         <v>25</v>
       </c>
@@ -4071,11 +3863,11 @@
       <c r="M13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
       <c r="S13" s="25" t="s">
         <v>25</v>
       </c>
@@ -4166,17 +3958,17 @@
       <c r="AV13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="AW13" s="27"/>
-      <c r="AX13" s="27"/>
-      <c r="AY13" s="29"/>
-      <c r="AZ13" s="29"/>
-      <c r="BA13" s="29"/>
-      <c r="BB13" s="29"/>
-      <c r="BC13" s="29"/>
-      <c r="BD13" s="29"/>
-      <c r="BE13" s="27"/>
-      <c r="BF13" s="27"/>
-      <c r="BH13" s="48"/>
+      <c r="AW13" s="33"/>
+      <c r="AX13" s="33"/>
+      <c r="AY13" s="32"/>
+      <c r="AZ13" s="32"/>
+      <c r="BA13" s="32"/>
+      <c r="BB13" s="32"/>
+      <c r="BC13" s="32"/>
+      <c r="BD13" s="32"/>
+      <c r="BE13" s="33"/>
+      <c r="BF13" s="33"/>
+      <c r="BH13" s="46"/>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
@@ -4249,7 +4041,7 @@
       <c r="BD14" s="11"/>
       <c r="BE14" s="6"/>
       <c r="BF14" s="6"/>
-      <c r="BH14" s="48"/>
+      <c r="BH14" s="46"/>
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
@@ -4318,7 +4110,7 @@
       <c r="BD15" s="13"/>
       <c r="BE15" s="7"/>
       <c r="BF15" s="7"/>
-      <c r="BH15" s="48"/>
+      <c r="BH15" s="46"/>
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -4387,7 +4179,7 @@
       <c r="BD16" s="11"/>
       <c r="BE16" s="6"/>
       <c r="BF16" s="6"/>
-      <c r="BH16" s="48"/>
+      <c r="BH16" s="46"/>
     </row>
     <row r="17" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
@@ -4456,7 +4248,7 @@
       <c r="BD17" s="12"/>
       <c r="BE17" s="9"/>
       <c r="BF17" s="9"/>
-      <c r="BH17" s="48"/>
+      <c r="BH17" s="46"/>
     </row>
     <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -4525,7 +4317,7 @@
       <c r="BD18" s="11"/>
       <c r="BE18" s="6"/>
       <c r="BF18" s="6"/>
-      <c r="BH18" s="48"/>
+      <c r="BH18" s="46"/>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
@@ -4594,7 +4386,7 @@
       <c r="BD19" s="9"/>
       <c r="BE19" s="9"/>
       <c r="BF19" s="9"/>
-      <c r="BH19" s="48"/>
+      <c r="BH19" s="46"/>
     </row>
     <row r="20" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
@@ -4663,7 +4455,7 @@
       <c r="BD20" s="11"/>
       <c r="BE20" s="6"/>
       <c r="BF20" s="6"/>
-      <c r="BH20" s="48"/>
+      <c r="BH20" s="46"/>
     </row>
     <row r="21" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
@@ -4732,35 +4524,35 @@
       <c r="BD21" s="9"/>
       <c r="BE21" s="9"/>
       <c r="BF21" s="9"/>
-      <c r="BH21" s="49"/>
+      <c r="BH21" s="47"/>
     </row>
     <row r="25" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="28" t="s">
+      <c r="F25" s="31" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
@@ -4889,6 +4681,56 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AZ1:AZ2"/>
+    <mergeCell ref="BB1:BB2"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AW1:AW2"/>
+    <mergeCell ref="AY1:AY2"/>
+    <mergeCell ref="BA1:BA2"/>
+    <mergeCell ref="BC1:BC2"/>
+    <mergeCell ref="AV1:AV2"/>
+    <mergeCell ref="AX1:AX2"/>
+    <mergeCell ref="AR1:AT1"/>
+    <mergeCell ref="AU1:AU2"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="AB12:AD12"/>
+    <mergeCell ref="AE12:AG12"/>
+    <mergeCell ref="AH12:AJ12"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="BF1:BF8"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="BF12:BF13"/>
+    <mergeCell ref="AW12:AW13"/>
+    <mergeCell ref="AX12:AX13"/>
+    <mergeCell ref="AY12:AY13"/>
+    <mergeCell ref="AZ12:AZ13"/>
+    <mergeCell ref="BA12:BA13"/>
     <mergeCell ref="BH12:BH21"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
@@ -4899,62 +4741,12 @@
     <mergeCell ref="BB12:BB13"/>
     <mergeCell ref="BC12:BC13"/>
     <mergeCell ref="BD12:BD13"/>
-    <mergeCell ref="BF1:BF8"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="BF12:BF13"/>
-    <mergeCell ref="AW12:AW13"/>
-    <mergeCell ref="AX12:AX13"/>
-    <mergeCell ref="AY12:AY13"/>
-    <mergeCell ref="AZ12:AZ13"/>
-    <mergeCell ref="BA12:BA13"/>
     <mergeCell ref="AK12:AM12"/>
     <mergeCell ref="AN12:AP12"/>
     <mergeCell ref="AQ12:AS12"/>
     <mergeCell ref="AT12:AV12"/>
     <mergeCell ref="V12:X12"/>
     <mergeCell ref="Y12:AA12"/>
-    <mergeCell ref="AB12:AD12"/>
-    <mergeCell ref="AE12:AG12"/>
-    <mergeCell ref="AH12:AJ12"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AV1:AV2"/>
-    <mergeCell ref="AX1:AX2"/>
-    <mergeCell ref="AR1:AT1"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AZ1:AZ2"/>
-    <mergeCell ref="BB1:BB2"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AW1:AW2"/>
-    <mergeCell ref="AY1:AY2"/>
-    <mergeCell ref="BA1:BA2"/>
-    <mergeCell ref="BC1:BC2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>